<commit_message>
Trum Update phân_công.xlsx ngày 9/10/2018 lúc 3:33PM
</commit_message>
<xml_diff>
--- a/phân_công.xlsx
+++ b/phân_công.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ka\Documents\VtcA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983D35F7-013D-44BA-936C-06E1AC4D3D3B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9768" windowHeight="3936" xr2:uid="{21E5FB16-10C4-459E-8C9C-87923E472F8F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9765" windowHeight="3930"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,31 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>làm animation player</t>
-  </si>
-  <si>
-    <t>làm animation cho đạn</t>
-  </si>
-  <si>
-    <t>viết physic cho đạn và barricade</t>
-  </si>
-  <si>
-    <t>làm pool đạn UI đạn cho súng AK</t>
-  </si>
-  <si>
-    <t>vật lý cho quái vật</t>
-  </si>
-  <si>
-    <t>respawn quái vật</t>
-  </si>
-  <si>
-    <t>máu, hiệu ứng tấn công và AI cho quái vật.</t>
-  </si>
-  <si>
-    <t>UI mua đồ</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Ka</t>
   </si>
@@ -77,14 +47,619 @@
     <t>Tú</t>
   </si>
   <si>
-    <t>Loading scene, start scene, item drop</t>
+    <t>*Nhân vật</t>
+  </si>
+  <si>
+    <t>*Zombie</t>
+  </si>
+  <si>
+    <t>*UI game, map và Item</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1)MAP GAME: làm theo or 
+sáng tạo </t>
+  </si>
+  <si>
+    <t>GHI CHÚ:</t>
+  </si>
+  <si>
+    <t>(2) Loading chuyển cảnh</t>
+  </si>
+  <si>
+    <t>(3) Show tiền khi kết thúc
+màn chơi làm theo or sáng tạo</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">11) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>UI trong game</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Setting, Shop, Súng, Skill, Tiền, Cây máu đại diện tổng số Zombie 1 cảnh, Máu của rào cản(2 cái cuối do a code, e tìm sprite cho a).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Animate zombie</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: đi, chạy, tấn công, tức giận, chết,...</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Animate:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nhân vật lúc bắn, thay đạn, lúc chết</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">9)   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Menu game</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">10) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Map game</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Loading chuyển cảnh</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Bảng show Tiền </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Xem ghi chú</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">12) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Các loại item bao gồm: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
++</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Các loại Súng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: AK, Shotgun, lửa, súng máy và quy định thông số tấn công cũng như thông số  nâng cấp cho từng loại  =&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tối thiểu 2 loại</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
++ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Các loại đạn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
++</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Skill nhân vậ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>t(lựu đạn nổ, lựu đạn băng, 1 loại làm chậm zombie, chất độc gây hút máu, 1 loại trở thành đồng minh của mình,...) =&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tối thiểu 2 loại</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
++ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tiền</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
++ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Máu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Damage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: bao gồm của các loại súng, các skill dựa vào thông số của Tú</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Animate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> hiệu ứng của các loại súng và skill</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nhà và 1 con pet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nếu được</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> để cho game sinh động or pet có skill
+càng tốt)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>7)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> HP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: bao gồm các loại Zombie, Boss và rào cản, HP đại diện số lượng zombie trong 1 màn chơi. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">8) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Damage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:  bao gồm các loại Zombie, Boss</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">9) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hiệu ứng</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> skill của 1 số zombie</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Số lượng Skill và Súng </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dựa vào số Sprite của Tú kiếm dc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">6) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Số lượng Skill </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tự kiếm</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +702,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -151,7 +748,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -228,17 +825,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color theme="2" tint="-0.499984740745262"/>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="2" tint="-0.499984740745262"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="thick">
-        <color theme="2" tint="-0.499984740745262"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
-      <top style="thick">
-        <color theme="2" tint="-0.499984740745262"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="thick">
-        <color theme="2" tint="-0.499984740745262"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -246,12 +852,101 @@
       <left style="thick">
         <color theme="2" tint="-0.499984740745262"/>
       </left>
-      <right/>
+      <right style="thick">
+        <color theme="2" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="2" tint="-0.499984740745262"/>
+      </left>
+      <right style="thick">
+        <color theme="2" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="2" tint="-0.499984740745262"/>
+      </left>
+      <right style="thick">
+        <color theme="2" tint="-0.499984740745262"/>
+      </right>
       <top style="thick">
         <color theme="2" tint="-0.499984740745262"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="2" tint="-0.499984740745262"/>
+      </left>
+      <right style="thick">
+        <color theme="2" tint="-0.499984740745262"/>
+      </right>
+      <top/>
       <bottom style="thick">
         <color theme="2" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="2" tint="-0.499984740745262"/>
+      </left>
+      <right style="thick">
+        <color theme="2" tint="-0.499984740745262"/>
+      </right>
+      <top style="thick">
+        <color theme="2" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -262,43 +957,81 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
@@ -319,6 +1052,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>182651</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7858125" y="952500"/>
+          <a:ext cx="4257675" cy="2459126"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9527</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7848602" y="3400426"/>
+          <a:ext cx="4276724" cy="2581274"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7839076" y="5991225"/>
+          <a:ext cx="4276724" cy="2743200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -364,7 +1234,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -416,7 +1286,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -610,123 +1480,196 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{902BAFB1-B853-4325-89F2-A3C03FF4769E}">
-  <dimension ref="A1:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="34.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" ht="34.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="26.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="21"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="22"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="22"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="22"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="22"/>
+    </row>
+    <row r="8" spans="1:4" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="10" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="10" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+      <c r="B13" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="8"/>
-      <c r="B6" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="24"/>
+    </row>
+    <row r="15" spans="1:4" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="8"/>
-      <c r="B10" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
+      <c r="C15" s="25"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="26"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="26"/>
+    </row>
+    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="11"/>
-    </row>
-    <row r="12" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="C18" s="26"/>
+    </row>
+    <row r="19" spans="1:3" ht="135" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="27"/>
+    </row>
+    <row r="20" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
+  <mergeCells count="4">
+    <mergeCell ref="A3:A8"/>
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>